<commit_message>
Make updates on cloture calcul
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_3_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_3_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -423,16 +423,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>001/test DR</v>
+        <v>001/DR IFRAN</v>
       </c>
       <c r="B2" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C2" t="str">
-        <v>123</v>
+        <v>DDDD</v>
       </c>
       <c r="D2" t="str">
-        <v>Yassine test</v>
+        <v>ALI EXPRESSE</v>
       </c>
       <c r="E2" t="str">
         <v>ds</v>
@@ -441,30 +441,112 @@
         <v>mensuelle</v>
       </c>
       <c r="G2">
-        <v>50000</v>
+        <v>12000</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>8000</v>
       </c>
       <c r="I2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J2">
-        <v>7500</v>
+        <v>1200</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="M2">
-        <v>42500</v>
+        <v>10800</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>001/DR IFRAN</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C3" t="str">
+        <v>BB132345</v>
+      </c>
+      <c r="D3" t="str">
+        <v>KHALID TAGHMAOUI</v>
+      </c>
+      <c r="E3" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F3" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G3">
+        <v>9000</v>
+      </c>
+      <c r="H3">
+        <v>6000</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>900</v>
+      </c>
+      <c r="K3">
+        <v>600</v>
+      </c>
+      <c r="L3">
+        <v>3000</v>
+      </c>
+      <c r="M3">
+        <v>8100</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>001/DR IFRAN</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C4" t="str">
+        <v>KS123456</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Youssef You</v>
+      </c>
+      <c r="E4" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F4" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G4">
+        <v>9000</v>
+      </c>
+      <c r="H4">
+        <v>6000</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <v>900</v>
+      </c>
+      <c r="K4">
+        <v>600</v>
+      </c>
+      <c r="L4">
+        <v>3000</v>
+      </c>
+      <c r="M4">
+        <v>8100</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix cloture calcul issues:
- add a condition if < date fin contrat > was null
- calculate < montant global brut / taxe > to each mondataire
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_3_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_3_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -441,7 +441,7 @@
         <v>mensuelle</v>
       </c>
       <c r="G2">
-        <v>12000</v>
+        <v>4000</v>
       </c>
       <c r="H2">
         <v>8000</v>
@@ -450,7 +450,7 @@
         <v>10</v>
       </c>
       <c r="J2">
-        <v>1200</v>
+        <v>400</v>
       </c>
       <c r="K2">
         <v>800</v>
@@ -459,7 +459,7 @@
         <v>4000</v>
       </c>
       <c r="M2">
-        <v>10800</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="3">
@@ -482,7 +482,7 @@
         <v>mensuelle</v>
       </c>
       <c r="G3">
-        <v>9000</v>
+        <v>3000</v>
       </c>
       <c r="H3">
         <v>6000</v>
@@ -491,7 +491,7 @@
         <v>10</v>
       </c>
       <c r="J3">
-        <v>900</v>
+        <v>300</v>
       </c>
       <c r="K3">
         <v>600</v>
@@ -500,7 +500,7 @@
         <v>3000</v>
       </c>
       <c r="M3">
-        <v>8100</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="4">
@@ -523,7 +523,7 @@
         <v>mensuelle</v>
       </c>
       <c r="G4">
-        <v>9000</v>
+        <v>3000</v>
       </c>
       <c r="H4">
         <v>6000</v>
@@ -532,7 +532,7 @@
         <v>10</v>
       </c>
       <c r="J4">
-        <v>900</v>
+        <v>300</v>
       </c>
       <c r="K4">
         <v>600</v>
@@ -541,12 +541,176 @@
         <v>3000</v>
       </c>
       <c r="M4">
-        <v>8100</v>
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>001/LF/DR IFRAN</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Logement de fonction</v>
+      </c>
+      <c r="C5" t="str">
+        <v>BB12354</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Tawfiq MF</v>
+      </c>
+      <c r="E5" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F5" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G5">
+        <v>1000</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>1000</v>
+      </c>
+      <c r="M5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>001/LF/DR IFRAN</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Logement de fonction</v>
+      </c>
+      <c r="C6" t="str">
+        <v>BB123456</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Ahmed tawfiq</v>
+      </c>
+      <c r="E6" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F6" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G6">
+        <v>2000</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>2000</v>
+      </c>
+      <c r="M6">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>001/LF/DR IFRAN</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Logement de fonction</v>
+      </c>
+      <c r="C7" t="str">
+        <v>bs3</v>
+      </c>
+      <c r="D7" t="str">
+        <v>IBM</v>
+      </c>
+      <c r="E7" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F7" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G7">
+        <v>3000</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>300</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>3000</v>
+      </c>
+      <c r="M7">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>001/LF/DR IFRAN</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Logement de fonction</v>
+      </c>
+      <c r="C8" t="str">
+        <v>BB123459</v>
+      </c>
+      <c r="D8" t="str">
+        <v>mamadu sacko</v>
+      </c>
+      <c r="E8" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F8" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G8">
+        <v>4000</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <v>400</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>4000</v>
+      </c>
+      <c r="M8">
+        <v>3600</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix uneditable situation cloture changes
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_3_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_3_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -708,9 +708,35 @@
         <v>3600</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>001/LF/DR IFRAN</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Logement de fonction</v>
+      </c>
+      <c r="C9" t="str">
+        <v>mdkjhf</v>
+      </c>
+      <c r="D9" t="str">
+        <v>test test</v>
+      </c>
+      <c r="E9" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F9" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Create updateProfile function :
- Add updateProfile function to put roles file
- Add updateProfile function route
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_3_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_3_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -444,22 +444,7 @@
         <v>4000</v>
       </c>
       <c r="H2">
-        <v>8000</v>
-      </c>
-      <c r="I2">
-        <v>10</v>
-      </c>
-      <c r="J2">
-        <v>400</v>
-      </c>
-      <c r="K2">
-        <v>800</v>
-      </c>
-      <c r="L2">
-        <v>4000</v>
-      </c>
-      <c r="M2">
-        <v>3600</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -734,9 +719,91 @@
         <v>0</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>123/Test SUP</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Supervision</v>
+      </c>
+      <c r="C10" t="str">
+        <v>BJ123456</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Hassan Hssouni</v>
+      </c>
+      <c r="E10" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F10" t="str">
+        <v>trimestrielle</v>
+      </c>
+      <c r="G10">
+        <v>100000</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>15</v>
+      </c>
+      <c r="J10">
+        <v>22500</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>50000</v>
+      </c>
+      <c r="M10">
+        <v>92500</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>002/DR002</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C11" t="str">
+        <v>cd1200</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Amine Kamal</v>
+      </c>
+      <c r="E11" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F11" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G11">
+        <v>40000</v>
+      </c>
+      <c r="H11">
+        <v>20000</v>
+      </c>
+      <c r="I11">
+        <v>15</v>
+      </c>
+      <c r="J11">
+        <v>3000</v>
+      </c>
+      <c r="K11">
+        <v>3000</v>
+      </c>
+      <c r="L11">
+        <v>20000</v>
+      </c>
+      <c r="M11">
+        <v>37000</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix orderVirement issue add <add banque_rib, ville_rib and cle_rib fields>
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_3_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_3_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -423,16 +423,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>001/DR IFRAN</v>
+        <v>001/LF/DR01</v>
       </c>
       <c r="B2" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C2" t="str">
-        <v>DDDD</v>
+        <v>BB196497</v>
       </c>
       <c r="D2" t="str">
-        <v>ALI EXPRESSE</v>
+        <v>Ahmed Taoufiq</v>
       </c>
       <c r="E2" t="str">
         <v>ds</v>
@@ -441,24 +441,39 @@
         <v>mensuelle</v>
       </c>
       <c r="G2">
-        <v>4000</v>
+        <v>30000</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>24000</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>2400</v>
+      </c>
+      <c r="K2">
+        <v>2400</v>
+      </c>
+      <c r="L2">
+        <v>6000</v>
+      </c>
+      <c r="M2">
+        <v>27600</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>001/DR IFRAN</v>
+        <v>001/LF/DR01</v>
       </c>
       <c r="B3" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C3" t="str">
-        <v>BB132345</v>
+        <v>BJ193607</v>
       </c>
       <c r="D3" t="str">
-        <v>KHALID TAGHMAOUI</v>
+        <v>Yassine AM</v>
       </c>
       <c r="E3" t="str">
         <v>ds</v>
@@ -467,343 +482,30 @@
         <v>mensuelle</v>
       </c>
       <c r="G3">
-        <v>3000</v>
+        <v>20000</v>
       </c>
       <c r="H3">
-        <v>6000</v>
+        <v>16000</v>
       </c>
       <c r="I3">
         <v>10</v>
       </c>
       <c r="J3">
-        <v>300</v>
+        <v>1600</v>
       </c>
       <c r="K3">
-        <v>600</v>
+        <v>1600</v>
       </c>
       <c r="L3">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="M3">
-        <v>2700</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>001/DR IFRAN</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="C4" t="str">
-        <v>KS123456</v>
-      </c>
-      <c r="D4" t="str">
-        <v>Youssef You</v>
-      </c>
-      <c r="E4" t="str">
-        <v>ds</v>
-      </c>
-      <c r="F4" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G4">
-        <v>3000</v>
-      </c>
-      <c r="H4">
-        <v>6000</v>
-      </c>
-      <c r="I4">
-        <v>10</v>
-      </c>
-      <c r="J4">
-        <v>300</v>
-      </c>
-      <c r="K4">
-        <v>600</v>
-      </c>
-      <c r="L4">
-        <v>3000</v>
-      </c>
-      <c r="M4">
-        <v>2700</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>001/LF/DR IFRAN</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Logement de fonction</v>
-      </c>
-      <c r="C5" t="str">
-        <v>BB12354</v>
-      </c>
-      <c r="D5" t="str">
-        <v>Tawfiq MF</v>
-      </c>
-      <c r="E5" t="str">
-        <v>ds</v>
-      </c>
-      <c r="F5" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G5">
-        <v>1000</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>1000</v>
-      </c>
-      <c r="M5">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>001/LF/DR IFRAN</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Logement de fonction</v>
-      </c>
-      <c r="C6" t="str">
-        <v>BB123456</v>
-      </c>
-      <c r="D6" t="str">
-        <v>Ahmed tawfiq</v>
-      </c>
-      <c r="E6" t="str">
-        <v>ds</v>
-      </c>
-      <c r="F6" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G6">
-        <v>2000</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>2000</v>
-      </c>
-      <c r="M6">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>001/LF/DR IFRAN</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Logement de fonction</v>
-      </c>
-      <c r="C7" t="str">
-        <v>bs3</v>
-      </c>
-      <c r="D7" t="str">
-        <v>IBM</v>
-      </c>
-      <c r="E7" t="str">
-        <v>ds</v>
-      </c>
-      <c r="F7" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G7">
-        <v>3000</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>10</v>
-      </c>
-      <c r="J7">
-        <v>300</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>3000</v>
-      </c>
-      <c r="M7">
-        <v>2700</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>001/LF/DR IFRAN</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Logement de fonction</v>
-      </c>
-      <c r="C8" t="str">
-        <v>BB123459</v>
-      </c>
-      <c r="D8" t="str">
-        <v>mamadu sacko</v>
-      </c>
-      <c r="E8" t="str">
-        <v>ds</v>
-      </c>
-      <c r="F8" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G8">
-        <v>4000</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>10</v>
-      </c>
-      <c r="J8">
-        <v>400</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>4000</v>
-      </c>
-      <c r="M8">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>001/LF/DR IFRAN</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Logement de fonction</v>
-      </c>
-      <c r="C9" t="str">
-        <v>mdkjhf</v>
-      </c>
-      <c r="D9" t="str">
-        <v>test test</v>
-      </c>
-      <c r="E9" t="str">
-        <v>ds</v>
-      </c>
-      <c r="F9" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>123/Test SUP</v>
-      </c>
-      <c r="B10" t="str">
-        <v>Supervision</v>
-      </c>
-      <c r="C10" t="str">
-        <v>BJ123456</v>
-      </c>
-      <c r="D10" t="str">
-        <v>Hassan Hssouni</v>
-      </c>
-      <c r="E10" t="str">
-        <v>ds</v>
-      </c>
-      <c r="F10" t="str">
-        <v>trimestrielle</v>
-      </c>
-      <c r="G10">
-        <v>100000</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>15</v>
-      </c>
-      <c r="J10">
-        <v>22500</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>50000</v>
-      </c>
-      <c r="M10">
-        <v>92500</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>002/DR002</v>
-      </c>
-      <c r="B11" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="C11" t="str">
-        <v>cd1200</v>
-      </c>
-      <c r="D11" t="str">
-        <v>Amine Kamal</v>
-      </c>
-      <c r="E11" t="str">
-        <v>ds</v>
-      </c>
-      <c r="F11" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G11">
-        <v>40000</v>
-      </c>
-      <c r="H11">
-        <v>20000</v>
-      </c>
-      <c r="I11">
-        <v>15</v>
-      </c>
-      <c r="J11">
-        <v>3000</v>
-      </c>
-      <c r="K11">
-        <v>3000</v>
-      </c>
-      <c r="L11">
-        <v>20000</v>
-      </c>
-      <c r="M11">
-        <v>37000</v>
+        <v>18400</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix code_lieu issue <situation cloture>
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_3_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_3_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -421,91 +421,9 @@
         <v>MT net</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>001/LF/DR01</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="C2" t="str">
-        <v>BB196497</v>
-      </c>
-      <c r="D2" t="str">
-        <v>Ahmed Taoufiq</v>
-      </c>
-      <c r="E2" t="str">
-        <v>ds</v>
-      </c>
-      <c r="F2" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G2">
-        <v>30000</v>
-      </c>
-      <c r="H2">
-        <v>24000</v>
-      </c>
-      <c r="I2">
-        <v>10</v>
-      </c>
-      <c r="J2">
-        <v>2400</v>
-      </c>
-      <c r="K2">
-        <v>2400</v>
-      </c>
-      <c r="L2">
-        <v>6000</v>
-      </c>
-      <c r="M2">
-        <v>27600</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>001/LF/DR01</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="C3" t="str">
-        <v>BJ193607</v>
-      </c>
-      <c r="D3" t="str">
-        <v>Yassine AM</v>
-      </c>
-      <c r="E3" t="str">
-        <v>ds</v>
-      </c>
-      <c r="F3" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G3">
-        <v>20000</v>
-      </c>
-      <c r="H3">
-        <v>16000</v>
-      </c>
-      <c r="I3">
-        <v>10</v>
-      </c>
-      <c r="J3">
-        <v>1600</v>
-      </c>
-      <c r="K3">
-        <v>1600</v>
-      </c>
-      <c r="L3">
-        <v>4000</v>
-      </c>
-      <c r="M3">
-        <v>18400</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add statut to post proprietaire
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_3_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_3_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -462,9 +462,132 @@
         <v>30000</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>120/SUP 2</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Supervision</v>
+      </c>
+      <c r="C3" t="str">
+        <v>O3546845</v>
+      </c>
+      <c r="D3" t="str">
+        <v xml:space="preserve">KHALID VAVA </v>
+      </c>
+      <c r="E3" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F3" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G3">
+        <v>18000</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>9000</v>
+      </c>
+      <c r="M3">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>120/SUP 2</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Supervision</v>
+      </c>
+      <c r="C4" t="str">
+        <v>L3659652</v>
+      </c>
+      <c r="D4" t="str">
+        <v>FATIMA FAFA</v>
+      </c>
+      <c r="E4" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F4" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G4">
+        <v>12000</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <v>600</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>6000</v>
+      </c>
+      <c r="M4">
+        <v>11400</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>001/CASA NORD</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C5" t="str">
+        <v>K6546841</v>
+      </c>
+      <c r="D5" t="str">
+        <v>IMANE FAFA</v>
+      </c>
+      <c r="E5" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F5" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G5">
+        <v>48000</v>
+      </c>
+      <c r="H5">
+        <v>36000</v>
+      </c>
+      <c r="I5">
+        <v>15</v>
+      </c>
+      <c r="J5">
+        <v>5400</v>
+      </c>
+      <c r="K5">
+        <v>5400</v>
+      </c>
+      <c r="L5">
+        <v>12000</v>
+      </c>
+      <c r="M5">
+        <v>42600</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix template taxe issue
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_3_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_3_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -585,9 +585,214 @@
         <v>42600</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>800/RABAT AGDAL</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C6" t="str">
+        <v>K2546546</v>
+      </c>
+      <c r="D6" t="str">
+        <v>KHADIJA PAPA</v>
+      </c>
+      <c r="E6" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F6" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G6">
+        <v>12000</v>
+      </c>
+      <c r="H6">
+        <v>9000</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <v>900</v>
+      </c>
+      <c r="K6">
+        <v>900</v>
+      </c>
+      <c r="L6">
+        <v>3000</v>
+      </c>
+      <c r="M6">
+        <v>11100</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>800/RABAT AGDAL</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C7" t="str">
+        <v>LP354654</v>
+      </c>
+      <c r="D7" t="str">
+        <v>SAAD NABIL</v>
+      </c>
+      <c r="E7" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F7" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G7">
+        <v>12000</v>
+      </c>
+      <c r="H7">
+        <v>9000</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>900</v>
+      </c>
+      <c r="K7">
+        <v>900</v>
+      </c>
+      <c r="L7">
+        <v>3000</v>
+      </c>
+      <c r="M7">
+        <v>11100</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>800/LF/RABAT AGDAL</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Logement de fonction</v>
+      </c>
+      <c r="C8" t="str">
+        <v>B3541456</v>
+      </c>
+      <c r="D8" t="str">
+        <v>JAJA GAGA</v>
+      </c>
+      <c r="E8" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F8" t="str">
+        <v>trimestrielle</v>
+      </c>
+      <c r="G8">
+        <v>28000</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <v>8400</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>25200</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>800/LF/RABAT AGDAL</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Logement de fonction</v>
+      </c>
+      <c r="C9" t="str">
+        <v>326546</v>
+      </c>
+      <c r="D9" t="str">
+        <v>STE CASA 56</v>
+      </c>
+      <c r="E9" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F9" t="str">
+        <v>trimestrielle</v>
+      </c>
+      <c r="G9">
+        <v>12000</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>622/CASA MEDINA</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Point de vente</v>
+      </c>
+      <c r="C10" t="str">
+        <v>G364861</v>
+      </c>
+      <c r="D10" t="str">
+        <v>MANAL LALA</v>
+      </c>
+      <c r="E10" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F10" t="str">
+        <v>annuelle</v>
+      </c>
+      <c r="G10">
+        <v>150000</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>15</v>
+      </c>
+      <c r="J10">
+        <v>270000</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>127500</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix siruation calcule issues
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_3_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_3_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -423,16 +423,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>903/CASA ANFA</v>
+        <v>512/CASA 2</v>
       </c>
       <c r="B2" t="str">
         <v>Point de vente</v>
       </c>
       <c r="C2" t="str">
-        <v>654566</v>
+        <v>31451</v>
       </c>
       <c r="D2" t="str">
-        <v>STT22</v>
+        <v xml:space="preserve">STE LOCATION </v>
       </c>
       <c r="E2" t="str">
         <v>ds</v>
@@ -441,10 +441,10 @@
         <v>mensuelle</v>
       </c>
       <c r="G2">
-        <v>30000</v>
+        <v>5000</v>
       </c>
       <c r="H2">
-        <v>15000</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -456,24 +456,24 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>15000</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>30000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>120/SUP 2</v>
+        <v>512/CASA 2</v>
       </c>
       <c r="B3" t="str">
-        <v>Supervision</v>
+        <v>Point de vente</v>
       </c>
       <c r="C3" t="str">
-        <v>O3546845</v>
+        <v>56987</v>
       </c>
       <c r="D3" t="str">
-        <v xml:space="preserve">KHALID VAVA </v>
+        <v xml:space="preserve">STE MAISON </v>
       </c>
       <c r="E3" t="str">
         <v>ds</v>
@@ -482,7 +482,7 @@
         <v>mensuelle</v>
       </c>
       <c r="G3">
-        <v>18000</v>
+        <v>5000</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -497,24 +497,24 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>9000</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>18000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>120/SUP 2</v>
+        <v>903/CASA ANFA/AV</v>
       </c>
       <c r="B4" t="str">
-        <v>Supervision</v>
+        <v>Point de vente</v>
       </c>
       <c r="C4" t="str">
-        <v>L3659652</v>
+        <v>654566</v>
       </c>
       <c r="D4" t="str">
-        <v>FATIMA FAFA</v>
+        <v>STT22</v>
       </c>
       <c r="E4" t="str">
         <v>ds</v>
@@ -523,39 +523,39 @@
         <v>mensuelle</v>
       </c>
       <c r="G4">
-        <v>12000</v>
+        <v>30000</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="I4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>6000</v>
+        <v>15000</v>
       </c>
       <c r="M4">
-        <v>11400</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>001/CASA NORD</v>
+        <v>120/SUP 2</v>
       </c>
       <c r="B5" t="str">
-        <v>Direction régionale</v>
+        <v>Supervision</v>
       </c>
       <c r="C5" t="str">
-        <v>K6546841</v>
+        <v>O3546845</v>
       </c>
       <c r="D5" t="str">
-        <v>IMANE FAFA</v>
+        <v xml:space="preserve">KHALID VAVA </v>
       </c>
       <c r="E5" t="str">
         <v>ds</v>
@@ -564,39 +564,39 @@
         <v>mensuelle</v>
       </c>
       <c r="G5">
-        <v>48000</v>
+        <v>18000</v>
       </c>
       <c r="H5">
-        <v>36000</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>5400</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>5400</v>
+        <v>0</v>
       </c>
       <c r="L5">
-        <v>12000</v>
+        <v>9000</v>
       </c>
       <c r="M5">
-        <v>42600</v>
+        <v>18000</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>800/RABAT AGDAL</v>
+        <v>120/SUP 2</v>
       </c>
       <c r="B6" t="str">
-        <v>Direction régionale</v>
+        <v>Supervision</v>
       </c>
       <c r="C6" t="str">
-        <v>K2546546</v>
+        <v>L3659652</v>
       </c>
       <c r="D6" t="str">
-        <v>KHADIJA PAPA</v>
+        <v>FATIMA FAFA</v>
       </c>
       <c r="E6" t="str">
         <v>ds</v>
@@ -608,36 +608,36 @@
         <v>12000</v>
       </c>
       <c r="H6">
-        <v>9000</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <v>10</v>
       </c>
       <c r="J6">
-        <v>900</v>
+        <v>600</v>
       </c>
       <c r="K6">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="L6">
-        <v>3000</v>
+        <v>6000</v>
       </c>
       <c r="M6">
-        <v>11100</v>
+        <v>11400</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>800/RABAT AGDAL</v>
+        <v>001/CASA NORD</v>
       </c>
       <c r="B7" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C7" t="str">
-        <v>LP354654</v>
+        <v>K6546841</v>
       </c>
       <c r="D7" t="str">
-        <v>SAAD NABIL</v>
+        <v>IMANE FAFA</v>
       </c>
       <c r="E7" t="str">
         <v>ds</v>
@@ -646,153 +646,235 @@
         <v>mensuelle</v>
       </c>
       <c r="G7">
+        <v>48000</v>
+      </c>
+      <c r="H7">
+        <v>36000</v>
+      </c>
+      <c r="I7">
+        <v>15</v>
+      </c>
+      <c r="J7">
+        <v>5400</v>
+      </c>
+      <c r="K7">
+        <v>5400</v>
+      </c>
+      <c r="L7">
         <v>12000</v>
       </c>
-      <c r="H7">
-        <v>9000</v>
-      </c>
-      <c r="I7">
-        <v>10</v>
-      </c>
-      <c r="J7">
-        <v>900</v>
-      </c>
-      <c r="K7">
-        <v>900</v>
-      </c>
-      <c r="L7">
-        <v>3000</v>
-      </c>
       <c r="M7">
-        <v>11100</v>
+        <v>42600</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>800/LF/RABAT AGDAL</v>
+        <v>800/RABAT AGDAL</v>
       </c>
       <c r="B8" t="str">
-        <v>Logement de fonction</v>
+        <v>Direction régionale</v>
       </c>
       <c r="C8" t="str">
-        <v>B3541456</v>
+        <v>K2546546</v>
       </c>
       <c r="D8" t="str">
-        <v>JAJA GAGA</v>
+        <v>KHADIJA PAPA</v>
       </c>
       <c r="E8" t="str">
         <v>ds</v>
       </c>
       <c r="F8" t="str">
-        <v>trimestrielle</v>
+        <v>mensuelle</v>
       </c>
       <c r="G8">
-        <v>28000</v>
+        <v>12000</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>9000</v>
       </c>
       <c r="I8">
         <v>10</v>
       </c>
       <c r="J8">
-        <v>8400</v>
+        <v>900</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="M8">
-        <v>25200</v>
+        <v>11100</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>800/LF/RABAT AGDAL</v>
+        <v>800/RABAT AGDAL</v>
       </c>
       <c r="B9" t="str">
-        <v>Logement de fonction</v>
+        <v>Direction régionale</v>
       </c>
       <c r="C9" t="str">
-        <v>326546</v>
+        <v>LP354654</v>
       </c>
       <c r="D9" t="str">
-        <v>STE CASA 56</v>
+        <v>SAAD NABIL</v>
       </c>
       <c r="E9" t="str">
         <v>ds</v>
       </c>
       <c r="F9" t="str">
-        <v>trimestrielle</v>
+        <v>mensuelle</v>
       </c>
       <c r="G9">
         <v>12000</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>9000</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="M9">
-        <v>12000</v>
+        <v>11100</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
+        <v>800/LF/RABAT AGDAL</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Logement de fonction</v>
+      </c>
+      <c r="C10" t="str">
+        <v>B3541456</v>
+      </c>
+      <c r="D10" t="str">
+        <v>JAJA GAGA</v>
+      </c>
+      <c r="E10" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F10" t="str">
+        <v>trimestrielle</v>
+      </c>
+      <c r="G10">
+        <v>28000</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>10</v>
+      </c>
+      <c r="J10">
+        <v>2800</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>25200</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>800/LF/RABAT AGDAL</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Logement de fonction</v>
+      </c>
+      <c r="C11" t="str">
+        <v>326546</v>
+      </c>
+      <c r="D11" t="str">
+        <v>STE CASA 56</v>
+      </c>
+      <c r="E11" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F11" t="str">
+        <v>trimestrielle</v>
+      </c>
+      <c r="G11">
+        <v>12000</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
         <v>622/CASA MEDINA</v>
       </c>
-      <c r="B10" t="str">
+      <c r="B12" t="str">
         <v>Point de vente</v>
       </c>
-      <c r="C10" t="str">
+      <c r="C12" t="str">
         <v>G364861</v>
       </c>
-      <c r="D10" t="str">
+      <c r="D12" t="str">
         <v>MANAL LALA</v>
       </c>
-      <c r="E10" t="str">
-        <v>ds</v>
-      </c>
-      <c r="F10" t="str">
+      <c r="E12" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F12" t="str">
         <v>annuelle</v>
       </c>
-      <c r="G10">
+      <c r="G12">
         <v>150000</v>
       </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
         <v>15</v>
       </c>
-      <c r="J10">
-        <v>270000</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
+      <c r="J12">
+        <v>22500</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
         <v>127500</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>